<commit_message>
Added more faces and practice run
</commit_message>
<xml_diff>
--- a/Encoding_Recall/UnusedNamesProf.xlsx
+++ b/Encoding_Recall/UnusedNamesProf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunduniversityo365-my.sharepoint.com/personal/em5456ol-s_lu_se/Documents/Jobb/Experiments/Faces_task/Gallerymemory/GalleryGame_block_fMRI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilo\OneDrive - Lund University\Jobb\Experiments\FacesNamesProfessions_fMRI\Encoding_Recall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC10489C71584F105BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7D8828A-A94D-49BA-A625-CCAE7D08AA0C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB634FF9-86AB-4ADC-A7E7-80835A14D10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="2970" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="92">
   <si>
     <t>Alt_2</t>
   </si>
@@ -92,9 +92,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>Filip</t>
-  </si>
-  <si>
     <t>"</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Tommy</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>Journalist</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>Tolk</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -161,18 +149,12 @@
     <t>W</t>
   </si>
   <si>
-    <t>IT-chef</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
     <t>Claes</t>
   </si>
   <si>
-    <t>Arkitekt</t>
-  </si>
-  <si>
     <t>Anton</t>
   </si>
   <si>
@@ -203,9 +185,6 @@
     <t>Kent</t>
   </si>
   <si>
-    <t>Rektor</t>
-  </si>
-  <si>
     <t>Ingvar</t>
   </si>
   <si>
@@ -218,12 +197,6 @@
     <t>Psykolog</t>
   </si>
   <si>
-    <t>Johannes</t>
-  </si>
-  <si>
-    <t>Konstnär</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -239,27 +212,15 @@
     <t>Jakob</t>
   </si>
   <si>
-    <t>Skådespelare</t>
-  </si>
-  <si>
     <t>Tobias</t>
   </si>
   <si>
-    <t>Djuruppfödare</t>
-  </si>
-  <si>
     <t>Lucas</t>
   </si>
   <si>
-    <t>Vetrinär</t>
-  </si>
-  <si>
     <t>Adam</t>
   </si>
   <si>
-    <t>Bagare</t>
-  </si>
-  <si>
     <t>Jonathan</t>
   </si>
   <si>
@@ -305,9 +266,6 @@
     <t>Kurt</t>
   </si>
   <si>
-    <t>Kemist</t>
-  </si>
-  <si>
     <t>Oliver</t>
   </si>
   <si>
@@ -323,73 +281,37 @@
     <t>Rune</t>
   </si>
   <si>
-    <t>Pilot</t>
-  </si>
-  <si>
-    <t>Isak</t>
-  </si>
-  <si>
     <t>PR-chef</t>
   </si>
   <si>
     <t>Georg</t>
   </si>
   <si>
-    <t>Präst</t>
-  </si>
-  <si>
     <t>Arvid</t>
   </si>
   <si>
-    <t>Politiker</t>
-  </si>
-  <si>
     <t>Ludvig</t>
   </si>
   <si>
-    <t>Officer</t>
-  </si>
-  <si>
-    <t>Gösta</t>
-  </si>
-  <si>
     <t>Torghandlare</t>
   </si>
   <si>
-    <t>Linus</t>
-  </si>
-  <si>
     <t>Ljudtekniker</t>
   </si>
   <si>
     <t>Johnny</t>
   </si>
   <si>
-    <t>Parkeringsvakt</t>
-  </si>
-  <si>
     <t>Albin</t>
   </si>
   <si>
-    <t>Apotekare</t>
-  </si>
-  <si>
     <t>Olle</t>
   </si>
   <si>
     <t>Butikssäljare</t>
   </si>
   <si>
-    <t>Edvin</t>
-  </si>
-  <si>
-    <t>Brandman</t>
-  </si>
-  <si>
     <t>Torbjörn</t>
-  </si>
-  <si>
-    <t>Managementkonsult</t>
   </si>
   <si>
     <t>Dan</t>
@@ -1028,7 +950,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K61"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,18 +1009,15 @@
       <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
       <c r="H2" t="str">
-        <f>LEFT(G2,1)</f>
-        <v>F</v>
+        <f t="shared" ref="H2:H41" si="0">LEFT(G2,1)</f>
+        <v/>
       </c>
       <c r="I2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2" t="str">
         <f>I2&amp;[1]Sheet1!E2&amp;J2</f>
@@ -1107,13 +1026,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -1122,20 +1041,17 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H3" t="str">
-        <f>LEFT(G3,1)</f>
-        <v>T</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" t="str">
         <f>I3&amp;[1]Sheet1!E3&amp;J3</f>
@@ -1147,32 +1063,32 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
       <c r="H4" t="str">
-        <f>LEFT(G4,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" t="str">
         <f>I4&amp;[1]Sheet1!E4&amp;J4</f>
@@ -1184,32 +1100,29 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
       <c r="H5" t="str">
-        <f>LEFT(G5,1)</f>
+        <f t="shared" si="0"/>
         <v>S</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5" t="str">
         <f>I5&amp;[1]Sheet1!E5&amp;J5</f>
@@ -1221,32 +1134,29 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
       <c r="H6" t="str">
-        <f>LEFT(G6,1)</f>
+        <f t="shared" si="0"/>
         <v>S</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" t="str">
         <f>I6&amp;[1]Sheet1!E6&amp;J6</f>
@@ -1258,32 +1168,29 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H7" t="str">
-        <f>LEFT(G7,1)</f>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" t="str">
         <f>I7&amp;[1]Sheet1!E7&amp;J7</f>
@@ -1292,35 +1199,32 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H8" t="str">
-        <f>LEFT(G8,1)</f>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K8" t="str">
         <f>I8&amp;[1]Sheet1!E8&amp;J8</f>
@@ -1329,35 +1233,35 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H9" t="str">
-        <f>LEFT(G9,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" t="str">
         <f>I9&amp;[1]Sheet1!E9&amp;J9</f>
@@ -1366,35 +1270,35 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H10" t="str">
-        <f>LEFT(G10,1)</f>
+        <f t="shared" si="0"/>
         <v>K</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K10" t="str">
         <f>I10&amp;[1]Sheet1!E10&amp;J10</f>
@@ -1403,35 +1307,32 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H11" t="str">
-        <f>LEFT(G11,1)</f>
+        <f t="shared" si="0"/>
         <v>I</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K11" t="str">
         <f>I11&amp;[1]Sheet1!E11&amp;J11</f>
@@ -1440,35 +1341,35 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H12" t="str">
-        <f>LEFT(G12,1)</f>
+        <f t="shared" si="0"/>
         <v>E</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K12" t="str">
         <f>I12&amp;[1]Sheet1!E12&amp;J12</f>
@@ -1477,35 +1378,32 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="H13" t="str">
-        <f>LEFT(G13,1)</f>
-        <v>J</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" t="str">
         <f>I13&amp;[1]Sheet1!E13&amp;J13</f>
@@ -1514,35 +1412,32 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H14" t="str">
-        <f>LEFT(G14,1)</f>
+        <f t="shared" si="0"/>
         <v>H</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K14" t="str">
         <f>I14&amp;[1]Sheet1!E14&amp;J14</f>
@@ -1551,35 +1446,35 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="H15" t="str">
-        <f>LEFT(G15,1)</f>
+        <f t="shared" si="0"/>
         <v>J</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K15" t="str">
         <f>I15&amp;[1]Sheet1!E15&amp;J15</f>
@@ -1593,30 +1488,27 @@
       <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="H16" t="str">
-        <f>LEFT(G16,1)</f>
+        <f t="shared" si="0"/>
         <v>T</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K16" t="str">
         <f>I16&amp;[1]Sheet1!E16&amp;J16</f>
@@ -1625,35 +1517,32 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="H17" t="str">
-        <f>LEFT(G17,1)</f>
+        <f t="shared" si="0"/>
         <v>L</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K17" t="str">
         <f>I17&amp;[1]Sheet1!E17&amp;J17</f>
@@ -1665,32 +1554,29 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="H18" t="str">
-        <f>LEFT(G18,1)</f>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K18" t="str">
         <f>I18&amp;[1]Sheet1!E18&amp;J18</f>
@@ -1699,35 +1585,32 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H19" t="str">
-        <f>LEFT(G19,1)</f>
+        <f t="shared" si="0"/>
         <v>J</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19" t="str">
         <f>I19&amp;[1]Sheet1!E19&amp;J19</f>
@@ -1736,35 +1619,35 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="H20" t="str">
-        <f>LEFT(G20,1)</f>
+        <f t="shared" si="0"/>
         <v>O</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K20" t="str">
         <f>I20&amp;[1]Sheet1!E20&amp;J20</f>
@@ -1773,35 +1656,35 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="H21" t="str">
-        <f>LEFT(G21,1)</f>
+        <f t="shared" si="0"/>
         <v>E</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K21" t="str">
         <f>I21&amp;[1]Sheet1!E21&amp;J21</f>
@@ -1810,35 +1693,35 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G22" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="H22" t="str">
-        <f>LEFT(G22,1)</f>
+        <f t="shared" si="0"/>
         <v>K</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K22" t="str">
         <f>I22&amp;[1]Sheet1!E22&amp;J22</f>
@@ -1847,35 +1730,35 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
         <v>19</v>
       </c>
-      <c r="F23" t="s">
-        <v>20</v>
-      </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="H23" t="str">
-        <f>LEFT(G23,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K23" t="str">
         <f>I23&amp;[1]Sheet1!E23&amp;J23</f>
@@ -1884,35 +1767,35 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="H24" t="str">
-        <f>LEFT(G24,1)</f>
+        <f t="shared" si="0"/>
         <v>J</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K24" t="str">
         <f>I24&amp;[1]Sheet1!E24&amp;J24</f>
@@ -1924,32 +1807,32 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
         <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="H25" t="str">
-        <f>LEFT(G25,1)</f>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K25" t="str">
         <f>I25&amp;[1]Sheet1!E25&amp;J25</f>
@@ -1958,13 +1841,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
@@ -1973,20 +1856,20 @@
         <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G26" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="H26" t="str">
-        <f>LEFT(G26,1)</f>
+        <f t="shared" si="0"/>
         <v>K</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K26" t="str">
         <f>I26&amp;[1]Sheet1!E26&amp;J26</f>
@@ -1995,35 +1878,32 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
         <v>39</v>
       </c>
-      <c r="C27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F27" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G27" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="H27" t="str">
-        <f>LEFT(G27,1)</f>
+        <f t="shared" si="0"/>
         <v>O</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K27" t="str">
         <f>I27&amp;[1]Sheet1!E27&amp;J27</f>
@@ -2032,35 +1912,35 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="H28" t="str">
-        <f>LEFT(G28,1)</f>
+        <f t="shared" si="0"/>
         <v>J</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K28" t="str">
         <f>I28&amp;[1]Sheet1!E28&amp;J28</f>
@@ -2069,35 +1949,35 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G29" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="H29" t="str">
-        <f>LEFT(G29,1)</f>
+        <f t="shared" si="0"/>
         <v>R</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K29" t="str">
         <f>I29&amp;[1]Sheet1!E29&amp;J29</f>
@@ -2109,32 +1989,26 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="H30" t="str">
-        <f>LEFT(G30,1)</f>
-        <v>I</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K30" t="str">
         <f>I30&amp;[1]Sheet1!E30&amp;J30</f>
@@ -2143,35 +2017,35 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
         <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G31" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="H31" t="str">
-        <f>LEFT(G31,1)</f>
+        <f t="shared" si="0"/>
         <v>G</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K31" t="str">
         <f>I31&amp;[1]Sheet1!E31&amp;J31</f>
@@ -2183,32 +2057,29 @@
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="D32" t="s">
         <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G32" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="H32" t="str">
-        <f>LEFT(G32,1)</f>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K32" t="str">
         <f>I32&amp;[1]Sheet1!E32&amp;J32</f>
@@ -2217,35 +2088,32 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
         <v>16</v>
       </c>
       <c r="G33" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="H33" t="str">
-        <f>LEFT(G33,1)</f>
+        <f t="shared" si="0"/>
         <v>L</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K33" t="str">
         <f>I33&amp;[1]Sheet1!E33&amp;J33</f>
@@ -2254,16 +2122,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
         <v>16</v>
       </c>
-      <c r="C34" t="s">
-        <v>102</v>
-      </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
         <v>16</v>
@@ -2271,18 +2136,15 @@
       <c r="F34" t="s">
         <v>11</v>
       </c>
-      <c r="G34" t="s">
-        <v>103</v>
-      </c>
       <c r="H34" t="str">
-        <f>LEFT(G34,1)</f>
-        <v>G</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K34" t="str">
         <f>I34&amp;[1]Sheet1!E34&amp;J34</f>
@@ -2291,35 +2153,32 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" t="s">
-        <v>105</v>
+        <v>19</v>
       </c>
       <c r="H35" t="str">
-        <f>LEFT(G35,1)</f>
-        <v>L</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K35" t="str">
         <f>I35&amp;[1]Sheet1!E35&amp;J35</f>
@@ -2328,35 +2187,35 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
         <v>22</v>
       </c>
-      <c r="B36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
       <c r="E36" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="H36" t="str">
-        <f>LEFT(G36,1)</f>
+        <f t="shared" si="0"/>
         <v>J</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K36" t="str">
         <f>I36&amp;[1]Sheet1!E36&amp;J36</f>
@@ -2365,35 +2224,32 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="D37" t="s">
         <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G37" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="H37" t="str">
-        <f>LEFT(G37,1)</f>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K37" t="str">
         <f>I37&amp;[1]Sheet1!E37&amp;J37</f>
@@ -2402,35 +2258,32 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E38" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F38" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G38" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="H38" t="str">
-        <f>LEFT(G38,1)</f>
+        <f t="shared" si="0"/>
         <v>O</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K38" t="str">
         <f>I38&amp;[1]Sheet1!E38&amp;J38</f>
@@ -2439,35 +2292,32 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" t="s">
         <v>27</v>
       </c>
-      <c r="C39" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" t="s">
-        <v>29</v>
-      </c>
       <c r="E39" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F39" t="s">
-        <v>47</v>
-      </c>
-      <c r="G39" t="s">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="H39" t="str">
-        <f>LEFT(G39,1)</f>
-        <v>E</v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K39" t="str">
         <f>I39&amp;[1]Sheet1!E39&amp;J39</f>
@@ -2479,32 +2329,29 @@
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G40" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="H40" t="str">
-        <f>LEFT(G40,1)</f>
+        <f t="shared" si="0"/>
         <v>T</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K40" t="str">
         <f>I40&amp;[1]Sheet1!E40&amp;J40</f>
@@ -2513,16 +2360,13 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2531,17 +2375,17 @@
         <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="H41" t="str">
-        <f>LEFT(G41,1)</f>
+        <f t="shared" si="0"/>
         <v>D</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K41" t="str">
         <f>I41&amp;[1]Sheet1!E41&amp;J41</f>
@@ -2550,16 +2394,16 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K42" t="str">
         <f>I42&amp;[1]Sheet1!E42&amp;J42</f>
@@ -2568,16 +2412,16 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K43" t="str">
         <f>I43&amp;[1]Sheet1!E43&amp;J43</f>
@@ -2586,16 +2430,16 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K44" t="str">
         <f>I44&amp;[1]Sheet1!E44&amp;J44</f>
@@ -2604,16 +2448,16 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K45" t="str">
         <f>I45&amp;[1]Sheet1!E45&amp;J45</f>
@@ -2622,16 +2466,16 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
         <v>22</v>
       </c>
-      <c r="B46" t="s">
-        <v>24</v>
-      </c>
       <c r="I46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K46" t="str">
         <f>I46&amp;[1]Sheet1!E46&amp;J46</f>
@@ -2640,16 +2484,16 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>52</v>
       </c>
-      <c r="B47" t="s">
-        <v>61</v>
-      </c>
       <c r="I47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K47" t="str">
         <f>I47&amp;[1]Sheet1!E47&amp;J47</f>
@@ -2658,16 +2502,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K48" t="str">
         <f>I48&amp;[1]Sheet1!E48&amp;J48</f>
@@ -2676,16 +2520,16 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K49" t="str">
         <f>I49&amp;[1]Sheet1!E49&amp;J49</f>
@@ -2694,13 +2538,13 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K50" t="str">
         <f>I50&amp;[1]Sheet1!E50&amp;J50</f>
@@ -2709,13 +2553,13 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K51" t="str">
         <f>I51&amp;[1]Sheet1!E51&amp;J51</f>
@@ -2724,13 +2568,13 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K52" t="str">
         <f>I52&amp;[1]Sheet1!E52&amp;J52</f>
@@ -2739,13 +2583,13 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K53" t="str">
         <f>I53&amp;[1]Sheet1!E53&amp;J53</f>
@@ -2754,13 +2598,13 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K54" t="str">
         <f>I54&amp;[1]Sheet1!E54&amp;J54</f>
@@ -2772,10 +2616,10 @@
         <v>14</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K55" t="str">
         <f>I55&amp;[1]Sheet1!E55&amp;J55</f>
@@ -2784,13 +2628,13 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K56" t="str">
         <f>I56&amp;[1]Sheet1!E56&amp;J56</f>
@@ -2799,13 +2643,13 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K57" t="str">
         <f>I57&amp;[1]Sheet1!E57&amp;J57</f>
@@ -2814,13 +2658,13 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K58" t="str">
         <f>I58&amp;[1]Sheet1!E58&amp;J58</f>
@@ -2829,13 +2673,13 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K59" t="str">
         <f>I59&amp;[1]Sheet1!E59&amp;J59</f>
@@ -2844,13 +2688,13 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K60" t="str">
         <f>I60&amp;[1]Sheet1!E60&amp;J60</f>
@@ -2862,10 +2706,10 @@
         <v>16</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K61" t="str">
         <f>I61&amp;[1]Sheet1!E61&amp;J61</f>

</xml_diff>